<commit_message>
temp.m - progressing on constraint definition
no longer using cvx
</commit_message>
<xml_diff>
--- a/fyp/matlab/importdata.xlsx
+++ b/fyp/matlab/importdata.xlsx
@@ -17,7 +17,6 @@
     <sheet name="k" sheetId="3" r:id="rId3"/>
     <sheet name="m" sheetId="4" r:id="rId4"/>
     <sheet name="misc" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>homes, hospital</t>
   </si>
@@ -97,13 +96,16 @@
     <t>k</t>
   </si>
   <si>
-    <t>rate</t>
-  </si>
-  <si>
     <t>flowPerCapitaPerDay</t>
   </si>
   <si>
     <t>pipeCostPerMetre</t>
+  </si>
+  <si>
+    <t>kA</t>
+  </si>
+  <si>
+    <t>backgroundConc</t>
   </si>
 </sst>
 </file>
@@ -125,7 +127,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,6 +137,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -177,7 +185,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -200,6 +208,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -857,15 +868,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -878,8 +889,14 @@
       <c r="D1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>17</v>
       </c>
@@ -892,8 +909,14 @@
       <c r="D2">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F2" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>18</v>
       </c>
@@ -906,8 +929,14 @@
       <c r="D3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3" s="2">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
@@ -919,6 +948,12 @@
       </c>
       <c r="D4">
         <v>30</v>
+      </c>
+      <c r="E4" s="10">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -938,10 +973,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -950,24 +985,6 @@
       </c>
       <c r="B2">
         <v>0.2218</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
used more meaningful variables
</commit_message>
<xml_diff>
--- a/fyp/matlab/importdata.xlsx
+++ b/fyp/matlab/importdata.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\cyeow.github.io\fyp\matlab\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7540" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7545" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="i" sheetId="1" r:id="rId1"/>
@@ -18,7 +13,7 @@
     <sheet name="m" sheetId="4" r:id="rId4"/>
     <sheet name="misc" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t>homes, hospital</t>
   </si>
@@ -66,15 +61,6 @@
     <t>treatmentTarget</t>
   </si>
   <si>
-    <t>Qk</t>
-  </si>
-  <si>
-    <t>Ak</t>
-  </si>
-  <si>
-    <t>ck</t>
-  </si>
-  <si>
     <t>population</t>
   </si>
   <si>
@@ -118,12 +104,18 @@
   </si>
   <si>
     <t>11b</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>flowCapacity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -285,7 +277,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -337,7 +329,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -531,7 +523,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -543,11 +535,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -559,7 +551,7 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
         <v>6</v>
@@ -854,15 +846,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -884,7 +876,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B3">
         <v>30.672630000000002</v>
@@ -895,7 +887,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B4">
         <v>30.66779</v>
@@ -917,7 +909,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>30.659030000000001</v>
@@ -928,7 +920,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>30.65249</v>
@@ -950,7 +942,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <v>30.657769999999999</v>
@@ -961,7 +953,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B10">
         <v>30.655999999999999</v>
@@ -990,22 +982,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -1087,15 +1081,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -1107,15 +1101,15 @@
         <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>155</v>
@@ -1124,7 +1118,7 @@
         <v>330</v>
       </c>
       <c r="D2">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="E2" s="2">
         <v>0.14000000000000001</v>
@@ -1135,7 +1129,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>26</v>
@@ -1144,7 +1138,7 @@
         <v>75</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="E3" s="2">
         <v>7.3999999999999996E-2</v>
@@ -1155,7 +1149,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>155</v>
@@ -1164,10 +1158,10 @@
         <v>286</v>
       </c>
       <c r="D4">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="E4" s="10">
-        <v>7.3999999999999996E-2</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
@@ -1183,17 +1177,17 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>